<commit_message>
Resultados consolidados depto -SG
</commit_message>
<xml_diff>
--- a/Frecuentista_depto/COL/Output/Tablas_resultado_teorico/IPM_teorico_vs_MC.xlsx
+++ b/Frecuentista_depto/COL/Output/Tablas_resultado_teorico/IPM_teorico_vs_MC.xlsx
@@ -467,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>0.500360563947559</v>
+        <v>0.491945396372404</v>
       </c>
       <c r="C2" t="n">
-        <v>0.500715891541389</v>
+        <v>0.49220524614661</v>
       </c>
     </row>
     <row r="3">
@@ -478,10 +478,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.443159196675601</v>
+        <v>0.455865178149482</v>
       </c>
       <c r="C3" t="n">
-        <v>0.443888069042572</v>
+        <v>0.454902509849823</v>
       </c>
     </row>
     <row r="4">
@@ -489,10 +489,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>0.280261798884935</v>
+        <v>0.255873391728952</v>
       </c>
       <c r="C4" t="n">
-        <v>0.276457930277781</v>
+        <v>0.256717934563359</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>0.643818202397916</v>
+        <v>0.630419104437875</v>
       </c>
       <c r="C5" t="n">
-        <v>0.642415226728463</v>
+        <v>0.630007896550884</v>
       </c>
     </row>
     <row r="6">
@@ -511,10 +511,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>0.647623254005529</v>
+        <v>0.659485831874964</v>
       </c>
       <c r="C6" t="n">
-        <v>0.647383251084125</v>
+        <v>0.660272612487221</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>0.518645259837972</v>
+        <v>0.540655018328467</v>
       </c>
       <c r="C7" t="n">
-        <v>0.518145547144133</v>
+        <v>0.542690479734615</v>
       </c>
     </row>
     <row r="8">
@@ -533,10 +533,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>0.788042611746126</v>
+        <v>0.737382789402442</v>
       </c>
       <c r="C8" t="n">
-        <v>0.789157990040742</v>
+        <v>0.735950890557437</v>
       </c>
     </row>
     <row r="9">
@@ -544,10 +544,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>0.798858635988069</v>
+        <v>0.786324640463071</v>
       </c>
       <c r="C9" t="n">
-        <v>0.799242586149413</v>
+        <v>0.786559537344948</v>
       </c>
     </row>
     <row r="10">
@@ -555,10 +555,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>0.654410008361485</v>
+        <v>0.63510138672369</v>
       </c>
       <c r="C10" t="n">
-        <v>0.653766840625008</v>
+        <v>0.635498627393652</v>
       </c>
     </row>
     <row r="11">
@@ -566,10 +566,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.729018813025103</v>
+        <v>0.734113151723734</v>
       </c>
       <c r="C11" t="n">
-        <v>0.732059470443295</v>
+        <v>0.7342148993472</v>
       </c>
     </row>
     <row r="12">
@@ -577,10 +577,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="n">
-        <v>0.526372553723191</v>
+        <v>0.534678276289036</v>
       </c>
       <c r="C12" t="n">
-        <v>0.523046801640699</v>
+        <v>0.534480549863145</v>
       </c>
     </row>
     <row r="13">
@@ -588,10 +588,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="n">
-        <v>0.941015646893282</v>
+        <v>0.949340103048975</v>
       </c>
       <c r="C13" t="n">
-        <v>0.940970895718239</v>
+        <v>0.949378946983765</v>
       </c>
     </row>
     <row r="14">
@@ -599,10 +599,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="n">
-        <v>0.586709184054661</v>
+        <v>0.56628802854227</v>
       </c>
       <c r="C14" t="n">
-        <v>0.587777492230615</v>
+        <v>0.566192776127786</v>
       </c>
     </row>
     <row r="15">
@@ -610,10 +610,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="n">
-        <v>0.830417738442631</v>
+        <v>0.814871237474843</v>
       </c>
       <c r="C15" t="n">
-        <v>0.832152042114255</v>
+        <v>0.815213495873063</v>
       </c>
     </row>
     <row r="16">
@@ -621,10 +621,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="n">
-        <v>0.733605533925808</v>
+        <v>0.700784933571959</v>
       </c>
       <c r="C16" t="n">
-        <v>0.732405967379009</v>
+        <v>0.698654908634361</v>
       </c>
     </row>
     <row r="17">
@@ -632,10 +632,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="n">
-        <v>0.585109846777274</v>
+        <v>0.635270097218214</v>
       </c>
       <c r="C17" t="n">
-        <v>0.587662154152059</v>
+        <v>0.637808022237456</v>
       </c>
     </row>
     <row r="18">
@@ -643,10 +643,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="n">
-        <v>0.828151842763659</v>
+        <v>0.836909470811762</v>
       </c>
       <c r="C18" t="n">
-        <v>0.827564719659073</v>
+        <v>0.839226701597952</v>
       </c>
     </row>
     <row r="19">
@@ -654,10 +654,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="n">
-        <v>0.635011999146189</v>
+        <v>0.645203803383275</v>
       </c>
       <c r="C19" t="n">
-        <v>0.63355969684019</v>
+        <v>0.645328115994307</v>
       </c>
     </row>
     <row r="20">
@@ -665,10 +665,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n">
-        <v>0.448029775436515</v>
+        <v>0.425471624783544</v>
       </c>
       <c r="C20" t="n">
-        <v>0.446511550281694</v>
+        <v>0.4254017981675</v>
       </c>
     </row>
     <row r="21">
@@ -676,10 +676,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="n">
-        <v>0.437395229619619</v>
+        <v>0.460626918026747</v>
       </c>
       <c r="C21" t="n">
-        <v>0.434902180648588</v>
+        <v>0.460150786390864</v>
       </c>
     </row>
     <row r="22">
@@ -687,10 +687,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="n">
-        <v>0.534284757327721</v>
+        <v>0.51612468554495</v>
       </c>
       <c r="C22" t="n">
-        <v>0.532068633312765</v>
+        <v>0.517378959828486</v>
       </c>
     </row>
     <row r="23">
@@ -698,10 +698,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="n">
-        <v>0.729630829197768</v>
+        <v>0.705839161308343</v>
       </c>
       <c r="C23" t="n">
-        <v>0.733717280465794</v>
+        <v>0.704527710256888</v>
       </c>
     </row>
     <row r="24">
@@ -709,10 +709,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>0.591959256324211</v>
+        <v>0.587123294766919</v>
       </c>
       <c r="C24" t="n">
-        <v>0.594123824117644</v>
+        <v>0.588589400461793</v>
       </c>
     </row>
     <row r="25">
@@ -720,10 +720,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="n">
-        <v>0.437039389051981</v>
+        <v>0.416354043259093</v>
       </c>
       <c r="C25" t="n">
-        <v>0.436127156003449</v>
+        <v>0.419346820527562</v>
       </c>
     </row>
     <row r="26">
@@ -731,10 +731,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="n">
-        <v>0.871097132454062</v>
+        <v>0.863622233182104</v>
       </c>
       <c r="C26" t="n">
-        <v>0.871020488917596</v>
+        <v>0.867860738206216</v>
       </c>
     </row>
     <row r="27">
@@ -742,10 +742,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="n">
-        <v>0.648413664136299</v>
+        <v>0.637928451019375</v>
       </c>
       <c r="C27" t="n">
-        <v>0.665751989870403</v>
+        <v>0.622679680185949</v>
       </c>
     </row>
     <row r="28">
@@ -753,10 +753,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n">
-        <v>0.868951595119737</v>
+        <v>0.862216976188318</v>
       </c>
       <c r="C28" t="n">
-        <v>0.879215507941192</v>
+        <v>0.874300338159811</v>
       </c>
     </row>
     <row r="29">
@@ -764,10 +764,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="n">
-        <v>0.860880844162319</v>
+        <v>0.855080362371329</v>
       </c>
       <c r="C29" t="n">
-        <v>0.866288727752142</v>
+        <v>0.852445616348055</v>
       </c>
     </row>
     <row r="30">
@@ -775,10 +775,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="n">
-        <v>0.959569962343995</v>
+        <v>0.956882332398853</v>
       </c>
       <c r="C30" t="n">
-        <v>0.955143512665637</v>
+        <v>0.94517020180737</v>
       </c>
     </row>
     <row r="31">
@@ -786,10 +786,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="n">
-        <v>0.964485773545521</v>
+        <v>0.962942446106548</v>
       </c>
       <c r="C31" t="n">
-        <v>0.961459538111405</v>
+        <v>0.961869939932097</v>
       </c>
     </row>
     <row r="32">
@@ -797,10 +797,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="n">
-        <v>0.861988530649484</v>
+        <v>0.856609675674819</v>
       </c>
       <c r="C32" t="n">
-        <v>0.846549276863467</v>
+        <v>0.848045421414048</v>
       </c>
     </row>
     <row r="33">
@@ -808,10 +808,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="n">
-        <v>0.979985099225999</v>
+        <v>0.980625221460318</v>
       </c>
       <c r="C33" t="n">
-        <v>0.978561581974616</v>
+        <v>0.981413699672006</v>
       </c>
     </row>
     <row r="34">
@@ -819,10 +819,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="n">
-        <v>0.95973975420605</v>
+        <v>0.956199985609417</v>
       </c>
       <c r="C34" t="n">
-        <v>0.952042778940249</v>
+        <v>0.956417897829349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>